<commit_message>
Atualização no site e sessão do simulador financeiro + daily dia 24/09
</commit_message>
<xml_diff>
--- a/documentacao/RequisitosPI.xlsx
+++ b/documentacao/RequisitosPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/projeto-pi-disel-2/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="13_ncr:1_{C25E80D5-3D1E-4FAF-8E3C-664635AE650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1335BAFC-0195-4366-8D61-1DC979B80295}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="13_ncr:1_{C25E80D5-3D1E-4FAF-8E3C-664635AE650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E9A36E3-2E7D-4172-8C91-DAA80D7AF1DC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="150">
   <si>
     <t>Requisito</t>
   </si>
@@ -620,9 +620,6 @@
   </si>
   <si>
     <t>Gustavo</t>
-  </si>
-  <si>
-    <t>Iniciar</t>
   </si>
   <si>
     <t>Vitor</t>
@@ -862,30 +859,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -906,6 +879,30 @@
     </xf>
     <xf numFmtId="14" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,7 +1291,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:C36"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1306,12 +1303,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -1690,7 +1687,7 @@
       <c r="F1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="35" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1713,7 +1710,7 @@
       <c r="F2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2066,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2088,88 +2085,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="13"/>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="M1" s="27" t="s">
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="M1" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="38">
         <v>45554</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="14"/>
       <c r="G2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="38">
         <v>45555</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
       <c r="M2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="28">
+      <c r="N2" s="38">
         <v>45557</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="15"/>
       <c r="G3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
       <c r="M3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -2202,13 +2199,13 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
       <c r="M5" s="8" t="s">
         <v>128</v>
       </c>
@@ -2225,11 +2222,11 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
       <c r="M6" s="8" t="s">
         <v>129</v>
       </c>
@@ -2246,11 +2243,11 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -2265,11 +2262,11 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -2300,37 +2297,37 @@
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="11" t="s">
         <v>103</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30" t="s">
+      <c r="H10" s="40"/>
+      <c r="I10" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="30"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30" t="s">
+      <c r="N10" s="40"/>
+      <c r="O10" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="P10" s="30"/>
+      <c r="P10" s="40"/>
       <c r="Q10" s="11" t="s">
         <v>103</v>
       </c>
@@ -2340,18 +2337,18 @@
         <v>104</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="12">
         <v>45560</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
       <c r="K11" s="12"/>
       <c r="M11" s="8" t="s">
         <v>104</v>
@@ -2372,18 +2369,18 @@
         <v>105</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="12">
         <v>45560</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
       <c r="K12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>105</v>
@@ -2404,18 +2401,18 @@
         <v>106</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="31"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="12">
         <v>45560</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
       <c r="K13" s="12"/>
       <c r="M13" s="8" t="s">
         <v>106</v>
@@ -2436,10 +2433,10 @@
         <v>109</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="12">
         <v>45560</v>
       </c>
@@ -2482,62 +2479,85 @@
       <c r="Q15" s="23"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="G16" s="27" t="s">
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="G16" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="M16" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="38">
         <v>45558</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
       <c r="G17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="38">
         <v>45559</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="M17" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N17" s="38">
+        <v>45560</v>
+      </c>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
       <c r="G18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H18" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="M18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>94</v>
       </c>
@@ -2552,8 +2572,15 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M19" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>134</v>
       </c>
@@ -2562,14 +2589,19 @@
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="G20" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>133</v>
       </c>
@@ -2578,14 +2610,19 @@
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="G21" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>135</v>
       </c>
@@ -2594,14 +2631,19 @@
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="G22" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -2612,8 +2654,13 @@
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>95</v>
       </c>
@@ -2628,12 +2675,19 @@
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
+      <c r="M24" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="30"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="24" t="s">
         <v>102</v>
       </c>
@@ -2643,10 +2697,10 @@
       <c r="E25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="H25" s="30"/>
+      <c r="H25" s="40"/>
       <c r="I25" s="24" t="s">
         <v>102</v>
       </c>
@@ -2656,121 +2710,152 @@
       <c r="K25" s="11" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="M25" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="27">
         <v>45560</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="G26" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="34" t="s">
+      <c r="H26" s="25"/>
+      <c r="I26" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="34" t="s">
+      <c r="J26" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="27">
         <v>45560</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="12"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="27">
         <v>45560</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G27" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="J27" s="34" t="s">
+      <c r="H27" s="25"/>
+      <c r="I27" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="J27" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="27">
         <v>45560</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="12"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9" t="s">
+      <c r="B28" s="28"/>
+      <c r="C28" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="30">
         <v>45560</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37" t="s">
+      <c r="H28" s="28"/>
+      <c r="I28" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="J28" s="37" t="s">
+      <c r="J28" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="K28" s="38">
+      <c r="K28" s="30">
         <v>45560</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="12"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="12">
+      <c r="D29" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="30">
         <v>45565</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40" t="s">
+      <c r="H29" s="31"/>
+      <c r="I29" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="J29" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="K29" s="41">
+      <c r="J29" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="K29" s="33">
         <v>45565</v>
       </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="39">
     <mergeCell ref="G16:K16"/>
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="H18:K18"/>
@@ -2802,6 +2887,14 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagrama de Solução(aguardando validação)
</commit_message>
<xml_diff>
--- a/documentacao/RequisitosPI.xlsx
+++ b/documentacao/RequisitosPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/projeto-pi-disel-2/documentacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-disel-2\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="13_ncr:1_{C25E80D5-3D1E-4FAF-8E3C-664635AE650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E9A36E3-2E7D-4172-8C91-DAA80D7AF1DC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D45D334-8FD8-416F-8FCB-B05D57ECFC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -886,23 +886,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,15 +1294,15 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>107</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>16</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>17</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>4</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>23</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>5</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>6</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>13</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>126</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>18</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>7</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>9</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>10</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>11</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>12</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>20</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>21</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>113</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>114</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>115</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>116</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>117</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>118</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>119</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>120</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>121</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>122</v>
       </c>
@@ -1663,12 +1663,12 @@
       <selection activeCell="A7" sqref="A7:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="15.77734375" customWidth="1"/>
+    <col min="1" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="G2" s="35"/>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>45</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>49</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>53</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>57</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>65</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>69</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>72</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>76</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>87</v>
       </c>
@@ -2063,112 +2063,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="3.44140625" customWidth="1"/>
-    <col min="7" max="9" width="13.77734375" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" customWidth="1"/>
-    <col min="12" max="12" width="3.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" customWidth="1"/>
-    <col min="16" max="16" width="20.21875" customWidth="1"/>
-    <col min="17" max="17" width="15.77734375" customWidth="1"/>
+    <col min="1" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="13"/>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="M1" s="37" t="s">
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="M1" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="37">
         <v>45554</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="14"/>
       <c r="G2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="37">
         <v>45555</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
       <c r="M2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="38">
+      <c r="N2" s="37">
         <v>45557</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="15"/>
       <c r="G3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
       <c r="M3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>94</v>
       </c>
@@ -2191,7 +2192,7 @@
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>98</v>
       </c>
@@ -2199,13 +2200,13 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
       <c r="M5" s="8" t="s">
         <v>128</v>
       </c>
@@ -2214,7 +2215,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>97</v>
       </c>
@@ -2222,11 +2223,11 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
       <c r="M6" s="8" t="s">
         <v>129</v>
       </c>
@@ -2235,7 +2236,7 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>99</v>
       </c>
@@ -2243,18 +2244,18 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>100</v>
       </c>
@@ -2262,18 +2263,18 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>95</v>
       </c>
@@ -2296,59 +2297,59 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="11" t="s">
         <v>103</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40" t="s">
+      <c r="H10" s="39"/>
+      <c r="I10" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="40"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40" t="s">
+      <c r="N10" s="39"/>
+      <c r="O10" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="P10" s="40"/>
+      <c r="P10" s="39"/>
       <c r="Q10" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>104</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="12">
         <v>45560</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
       <c r="K11" s="12"/>
       <c r="M11" s="8" t="s">
         <v>104</v>
@@ -2364,23 +2365,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>105</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="12">
         <v>45560</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
       <c r="K12" s="12"/>
       <c r="M12" s="8" t="s">
         <v>105</v>
@@ -2396,23 +2397,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>106</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="12">
         <v>45560</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
       <c r="K13" s="12"/>
       <c r="M13" s="8" t="s">
         <v>106</v>
@@ -2428,15 +2429,15 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="12">
         <v>45560</v>
       </c>
@@ -2459,7 +2460,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -2478,86 +2479,86 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="G16" s="37" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="G16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="M16" s="37" t="s">
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="M16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="37">
         <v>45558</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
       <c r="G17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="37">
         <v>45559</v>
       </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
       <c r="M17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="N17" s="38">
+      <c r="N17" s="37">
         <v>45560</v>
       </c>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
       <c r="G18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="39" t="s">
+      <c r="H18" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
       <c r="M18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>94</v>
       </c>
@@ -2580,7 +2581,7 @@
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>134</v>
       </c>
@@ -2601,7 +2602,7 @@
       <c r="P20" s="22"/>
       <c r="Q20" s="22"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>133</v>
       </c>
@@ -2622,7 +2623,7 @@
       <c r="P21" s="22"/>
       <c r="Q21" s="22"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>135</v>
       </c>
@@ -2643,7 +2644,7 @@
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -2660,7 +2661,7 @@
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>95</v>
       </c>
@@ -2683,11 +2684,11 @@
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="40" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="24" t="s">
         <v>102</v>
       </c>
@@ -2697,10 +2698,10 @@
       <c r="E25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="40" t="s">
+      <c r="G25" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="H25" s="40"/>
+      <c r="H25" s="39"/>
       <c r="I25" s="24" t="s">
         <v>102</v>
       </c>
@@ -2710,19 +2711,19 @@
       <c r="K25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="M25" s="40" t="s">
+      <c r="M25" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40" t="s">
+      <c r="N25" s="39"/>
+      <c r="O25" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="P25" s="40"/>
+      <c r="P25" s="39"/>
       <c r="Q25" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>136</v>
       </c>
@@ -2751,11 +2752,11 @@
       </c>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="36"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
       <c r="Q26" s="12"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>105</v>
       </c>
@@ -2784,11 +2785,11 @@
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
       <c r="Q27" s="12"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>138</v>
       </c>
@@ -2817,11 +2818,11 @@
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
       <c r="Q28" s="12"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>142</v>
       </c>
@@ -2856,16 +2857,19 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G5:K8"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C11:D11"/>
@@ -2882,19 +2886,16 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G5:K8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização do CSS - pagina 2 simulador e acrescentando a página 3
</commit_message>
<xml_diff>
--- a/documentacao/RequisitosPI.xlsx
+++ b/documentacao/RequisitosPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-disel-2\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/projeto-pi-diesel-2/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83792C9-AA03-47B7-B1A9-83FE05156973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{B83792C9-AA03-47B7-B1A9-83FE05156973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53D23D6B-CF74-41EB-98CA-ABDAB6C0AEF1}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="2850" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="162">
   <si>
     <t>Requisito</t>
   </si>
@@ -629,9 +629,6 @@
     <t>Finalizado</t>
   </si>
   <si>
-    <t>* Comnetários sobre as tabelas/modelagem de nossa regra de negócio</t>
-  </si>
-  <si>
     <t>* Finalização do código do arduíno, focando somente no sensor ultrassônico</t>
   </si>
   <si>
@@ -639,6 +636,42 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Site institucional (HTML/JS/CSS)</t>
+  </si>
+  <si>
+    <t>Site (Área de login/cadastro)</t>
+  </si>
+  <si>
+    <t>Site (Área de dashboards)</t>
+  </si>
+  <si>
+    <t>Site (Área do Simulador)</t>
+  </si>
+  <si>
+    <t>Gustavo / Jin</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>Vitor / Guilherme</t>
+  </si>
+  <si>
+    <t>Iniciar</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>* Definições para a próxima semana</t>
+  </si>
+  <si>
+    <t>* Discussões sobre como seguir com o marketing do simulador financeiro</t>
+  </si>
+  <si>
+    <t>* Comentários sobre as tabelas/modelagem de nossa regra de negócio</t>
   </si>
 </sst>
 </file>
@@ -695,13 +728,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFC000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
@@ -721,6 +747,14 @@
       <b/>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -782,7 +816,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -790,11 +824,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -818,9 +893,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -849,17 +921,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -874,12 +947,26 @@
     <xf numFmtId="14" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -887,19 +974,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1295,339 +1394,339 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="74.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="17"/>
+      <c r="C29" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18" t="s">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18" t="s">
+      <c r="B33" s="17"/>
+      <c r="C33" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1664,12 +1763,12 @@
       <selection activeCell="A7" sqref="A7:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -1688,11 +1787,11 @@
       <c r="F1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1711,9 +1810,9 @@
       <c r="F2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="35"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
@@ -1736,7 +1835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>45</v>
       </c>
@@ -1759,7 +1858,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
@@ -1782,7 +1881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
@@ -1805,7 +1904,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>49</v>
       </c>
@@ -1826,7 +1925,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>53</v>
       </c>
@@ -1847,7 +1946,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>57</v>
       </c>
@@ -1868,7 +1967,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1889,7 +1988,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>65</v>
       </c>
@@ -1910,7 +2009,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>69</v>
       </c>
@@ -1931,7 +2030,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>72</v>
       </c>
@@ -1952,7 +2051,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>76</v>
       </c>
@@ -1973,7 +2072,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
@@ -1994,7 +2093,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2015,7 +2114,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>87</v>
       </c>
@@ -2064,136 +2163,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R38" sqref="R1:R1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="7" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
+    <col min="13" max="13" width="30.77734375" customWidth="1"/>
+    <col min="14" max="14" width="5" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="37" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="M1" s="37" t="s">
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="M1" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="43">
         <v>45554</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="14"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="43">
         <v>45555</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
       <c r="M2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="38">
+      <c r="N2" s="43">
         <v>45557</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="15"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
       <c r="M3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="G4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="M4" s="10" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="M4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>98</v>
       </c>
@@ -2201,13 +2302,13 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
       <c r="M5" s="8" t="s">
         <v>128</v>
       </c>
@@ -2216,7 +2317,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>97</v>
       </c>
@@ -2224,11 +2325,11 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
       <c r="M6" s="8" t="s">
         <v>129</v>
       </c>
@@ -2237,7 +2338,7 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>99</v>
       </c>
@@ -2245,18 +2346,18 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>100</v>
       </c>
@@ -2264,182 +2365,182 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="G9" s="10" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="G9" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="M9" s="10" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="M9" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="40" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40" t="s">
+      <c r="H10" s="45"/>
+      <c r="I10" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="11" t="s">
+      <c r="J10" s="45"/>
+      <c r="K10" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40" t="s">
+      <c r="N10" s="45"/>
+      <c r="O10" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="11" t="s">
+      <c r="P10" s="45"/>
+      <c r="Q10" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="12">
+      <c r="D11" s="46"/>
+      <c r="E11" s="36">
         <v>45560</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="12"/>
-      <c r="M11" s="8" t="s">
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="11"/>
+      <c r="M11" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9" t="s">
+      <c r="N11" s="25"/>
+      <c r="O11" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="Q11" s="12">
+      <c r="Q11" s="27">
         <v>45560</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="36" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="12">
+      <c r="D12" s="46"/>
+      <c r="E12" s="36">
         <v>45560</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="12"/>
-      <c r="M12" s="8" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="11"/>
+      <c r="M12" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9" t="s">
+      <c r="N12" s="22"/>
+      <c r="O12" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="P12" s="21" t="s">
+      <c r="P12" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="Q12" s="24">
         <v>45560</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="36" t="s">
+      <c r="B13" s="41"/>
+      <c r="C13" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="12">
+      <c r="D13" s="46"/>
+      <c r="E13" s="36">
         <v>45560</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="12"/>
-      <c r="M13" s="8" t="s">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="11"/>
+      <c r="M13" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="9" t="s">
+      <c r="N13" s="22"/>
+      <c r="O13" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="Q13" s="24">
         <v>45560</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="36" t="s">
+      <c r="B14" s="41"/>
+      <c r="C14" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="12">
+      <c r="D14" s="46"/>
+      <c r="E14" s="36">
         <v>45560</v>
       </c>
       <c r="G14" s="8"/>
@@ -2447,361 +2548,385 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="9" t="s">
+      <c r="N14" s="25"/>
+      <c r="O14" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="P14" s="20" t="s">
+      <c r="P14" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="27">
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="G16" s="37" t="s">
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="G16" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="M16" s="37" t="s">
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="M16" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="43">
         <v>45558</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
       <c r="G17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="43">
         <v>45559</v>
       </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
       <c r="M17" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="N17" s="38">
+      <c r="N17" s="43">
         <v>45560</v>
       </c>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
       <c r="G18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="39" t="s">
+      <c r="H18" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
       <c r="M18" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="N18" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="G19" s="10" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="G19" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="M19" s="10" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="M19" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="G20" s="22" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="G20" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="M20" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="G21" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="G21" s="22" t="s">
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="M21" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="G22" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="G22" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="G24" s="10" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="G24" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="M24" s="10" t="s">
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="M24" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="24" t="s">
+      <c r="B25" s="45"/>
+      <c r="C25" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="40" t="s">
+      <c r="G25" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="24" t="s">
+      <c r="H25" s="45"/>
+      <c r="I25" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="J25" s="24" t="s">
+      <c r="J25" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="M25" s="40" t="s">
+      <c r="M25" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40" t="s">
+      <c r="N25" s="45"/>
+      <c r="O25" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="11" t="s">
+      <c r="P25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q25" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="24">
         <v>45560</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="26" t="s">
+      <c r="H26" s="28"/>
+      <c r="I26" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="K26" s="30">
+        <v>45560</v>
+      </c>
+      <c r="M26" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="P26" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q26" s="32">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="K26" s="27">
+      <c r="E27" s="24">
         <v>45560</v>
       </c>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="12"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="G27" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26" t="s">
+      <c r="H27" s="28"/>
+      <c r="I27" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="27">
+      <c r="J27" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="K27" s="30">
         <v>45560</v>
       </c>
-      <c r="G27" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="J27" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="K27" s="27">
-        <v>45560</v>
-      </c>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="12"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="M27" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="P27" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q27" s="32">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29" t="s">
+      <c r="B28" s="25"/>
+      <c r="C28" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="27">
         <v>45560</v>
       </c>
       <c r="G28" s="28" t="s">
@@ -2812,96 +2937,157 @@
         <v>139</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="K28" s="30">
         <v>45560</v>
       </c>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="12"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="M28" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="P28" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q28" s="32">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="27">
         <v>45565</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32" t="s">
+      <c r="H29" s="28"/>
+      <c r="I29" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J29" s="32" t="s">
+      <c r="J29" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="K29" s="33">
+      <c r="K29" s="30">
         <v>45565</v>
       </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-    </row>
-    <row r="59" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="M29" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="P29" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q29" s="32">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="M30" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="P30" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q30" s="34">
+        <v>45561</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+    </row>
+    <row r="59" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G5:K8"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="O10:P10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G5:K8"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="M25:N25"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="M16:Q16"/>
     <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização no simulador financeiro + planilha de backlog
</commit_message>
<xml_diff>
--- a/documentacao/RequisitosPI.xlsx
+++ b/documentacao/RequisitosPI.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/projeto-pi-diesel-2/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{B83792C9-AA03-47B7-B1A9-83FE05156973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53D23D6B-CF74-41EB-98CA-ABDAB6C0AEF1}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="13_ncr:1_{B83792C9-AA03-47B7-B1A9-83FE05156973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DCBC797-3F66-4D2A-AB94-97AD4F0C6EAF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
     <sheet name="5W2H" sheetId="2" r:id="rId2"/>
     <sheet name="Dayli" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BackLog!$A$2:$I$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="191">
   <si>
     <t>Requisito</t>
   </si>
@@ -47,48 +50,12 @@
     <t>Classificação</t>
   </si>
   <si>
-    <t>Calculadora Financeira</t>
-  </si>
-  <si>
-    <t>Backend - integrado com banco de dados e API e Dash board</t>
-  </si>
-  <si>
-    <t>Protótipo do site institucional apresentado no Canva e/ou Figma</t>
-  </si>
-  <si>
-    <t>URL contendo o simulador financeiro finalizado</t>
-  </si>
-  <si>
-    <t>Diagrama da Solução de Projeto</t>
-  </si>
-  <si>
     <t>Diagrama de Visão de Negócio</t>
   </si>
   <si>
     <t>Planilha de backlog</t>
   </si>
   <si>
-    <t>Finalização site institucional</t>
-  </si>
-  <si>
-    <t>Integração da coleta de dados do sensor com o banco de dados</t>
-  </si>
-  <si>
-    <t>Incrementos na documentação do projeto</t>
-  </si>
-  <si>
-    <t>Tabelas criadas para o banco de dados, no MySQL</t>
-  </si>
-  <si>
-    <t>Home Page</t>
-  </si>
-  <si>
-    <t>Tela de login com senha</t>
-  </si>
-  <si>
-    <t>Tela de cadastro</t>
-  </si>
-  <si>
     <t>Tela de Contato e suporte</t>
   </si>
   <si>
@@ -108,9 +75,6 @@
   </si>
   <si>
     <t>Documento de Contexto de Negócio e Justificativa do Projeto</t>
-  </si>
-  <si>
-    <t>Script das tabelas</t>
   </si>
   <si>
     <t>Instalação e Configuração IDE Arduíno</t>
@@ -527,36 +491,15 @@
     <t>Vitor/Gustavo</t>
   </si>
   <si>
-    <t>Atualização do projeto no GitHub / Documentação</t>
-  </si>
-  <si>
     <t>Planilha de riscos do Projeto</t>
   </si>
   <si>
-    <t>Especificação da DashBoard</t>
-  </si>
-  <si>
     <t>Site estático Institucional - Local em HTML / CSS / JS</t>
   </si>
   <si>
-    <t>Site estático DashBoard</t>
-  </si>
-  <si>
-    <t>Site estático Cadastro e Login</t>
-  </si>
-  <si>
     <t>Diagrama de solução</t>
   </si>
   <si>
-    <t>Modelagem Lógica do Projeto v1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Script de criação do banco </t>
-  </si>
-  <si>
-    <t>Instalar MySQL na VMLinux e inserção de dados do Arduíno</t>
-  </si>
-  <si>
     <t>Desejável</t>
   </si>
   <si>
@@ -566,9 +509,6 @@
     <t>Importante</t>
   </si>
   <si>
-    <t>Ligar Arduino e executar Código com o sensor ultrassônico</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reunião remarcada para domingo, devido necessidade do grupo </t>
   </si>
   <si>
@@ -672,6 +612,156 @@
   </si>
   <si>
     <t>* Comentários sobre as tabelas/modelagem de nossa regra de negócio</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Tam (#)</t>
+  </si>
+  <si>
+    <t>Prioridade</t>
+  </si>
+  <si>
+    <t>SPRINT</t>
+  </si>
+  <si>
+    <t>Home Page (Protótipo)</t>
+  </si>
+  <si>
+    <t>Página institucional desenvolvida no Canva / Figma</t>
+  </si>
+  <si>
+    <t>Sessão do site estática para cadastro e login de usuários, com validação de caractéres</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>Projetos atualizado no GitHub / Documentação do Projeto Atualizada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualização de commits e continuação em partes importantes da documentação (backlog, requisitos...) </t>
+  </si>
+  <si>
+    <t>Área estática do site para manutenção futura do projeto</t>
+  </si>
+  <si>
+    <t>Planilha para orientar as inviabilidades do projetos e possíveis contra-tempos</t>
+  </si>
+  <si>
+    <t>Site estático DashBoard (Especificação)</t>
+  </si>
+  <si>
+    <t>Área do usuário que terá os recebimentos de dados monitorados pelo sensor ultrassônico</t>
+  </si>
+  <si>
+    <t>Site estático Institucional - Área de cadastro e Login</t>
+  </si>
+  <si>
+    <t>Site institucional já implementado com línguagens JS, HTML e CSS</t>
+  </si>
+  <si>
+    <t>Diagrama de solução do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama com solução técnica do projeto, de fácil entendimento de como será nossa atuação </t>
+  </si>
+  <si>
+    <t>Backlog da Sprint</t>
+  </si>
+  <si>
+    <t>Planilha para pontuar os principais requisitos do projeto e orientar itens de importância</t>
+  </si>
+  <si>
+    <t>Modelagem lógica do projeto</t>
+  </si>
+  <si>
+    <t>Modelagem do projeto, relacionando como as tabelas principais de dados irão se comunicar</t>
+  </si>
+  <si>
+    <t>Scripts das principais tabelas do projeto</t>
+  </si>
+  <si>
+    <t>Simular a integração do Sistema</t>
+  </si>
+  <si>
+    <t>Utilizar API do node.js para simular o recebimento de dados na área de dashboards do projeto</t>
+  </si>
+  <si>
+    <t>Usar API Local / Sensor</t>
+  </si>
+  <si>
+    <t>Uso da API fornecida para recebimento de dados</t>
+  </si>
+  <si>
+    <t>Instalação de MySQL na VM e inserção de dados</t>
+  </si>
+  <si>
+    <t>Inserção de dados no banco de dados a partir da máquina virtual</t>
+  </si>
+  <si>
+    <t>Simulador Financeiro</t>
+  </si>
+  <si>
+    <t>Área do site para apresentar o principal Marketing de nosso projeto</t>
+  </si>
+  <si>
+    <t>Script de criação do banco v2</t>
+  </si>
+  <si>
+    <t>Script das tabelas v1</t>
+  </si>
+  <si>
+    <t>Scripts iniciais do projeto sem relacionamento entre as tabelas</t>
+  </si>
+  <si>
+    <t>Criação inicial do projeto no GitHub</t>
+  </si>
+  <si>
+    <t>Primeira versão da documentação do projeto, com contextualização inicial, justificativa e objetivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama para apresentar de uma maneira geral como funciona nossa solução com um olhar de negócios </t>
+  </si>
+  <si>
+    <t>Ferramenta de gestão para auxilio das tarefas realizadas pela equipe</t>
+  </si>
+  <si>
+    <t>Configuração inicial do sensor na IDE do arduíno</t>
+  </si>
+  <si>
+    <t>Logo inicial da empresa para representar nossa marca empresarial</t>
+  </si>
+  <si>
+    <t>Paleta de cores que será utilizada para site e apresentação do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuração da VM que receberá futuros dados, em ambiente linux </t>
+  </si>
+  <si>
+    <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluxograma de Suporte </t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk</t>
+  </si>
+  <si>
+    <t>Documento de mudança</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluxograma que irá definir os caminhos de contato para suporte aos clientes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferramenta para auxilio de clientes </t>
+  </si>
+  <si>
+    <t>Documento para pontuar modificações e implementações de mudanças do projeto</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
   </si>
 </sst>
 </file>
@@ -717,19 +807,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -758,6 +835,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -869,7 +959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -912,20 +1002,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -933,30 +1028,16 @@
     <xf numFmtId="14" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -965,44 +1046,60 @@
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1387,354 +1484,577 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="74.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="D2" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+    </row>
+    <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+    </row>
+    <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+    </row>
+    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+    </row>
+    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+    </row>
+    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+    </row>
+    <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+    </row>
+    <row r="20" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+    </row>
+    <row r="21" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="B21" s="51" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="B25" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17" t="s">
-        <v>124</v>
+      <c r="B26" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+    </row>
+    <row r="27" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:I2" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="D2:I2 C2:C1048576">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"ESSENCIAL"</formula>
     </cfRule>
@@ -1746,7 +2066,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36" xr:uid="{C6A8AFFE-3DC7-45BF-9737-E7A938D030B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C26" xr:uid="{C6A8AFFE-3DC7-45BF-9737-E7A938D030B3}">
       <formula1>"Desejável, Essencial, Importante"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1770,369 +2090,369 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="39"/>
+        <v>25</v>
+      </c>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2163,7 +2483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
@@ -2188,106 +2508,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="A1" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="12"/>
-      <c r="G1" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="M1" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
+      <c r="G1" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="M1" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="43">
+        <v>79</v>
+      </c>
+      <c r="B2" s="37">
         <v>45554</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="13"/>
       <c r="G2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="43">
+        <v>79</v>
+      </c>
+      <c r="H2" s="37">
         <v>45555</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
       <c r="M2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" s="43">
+        <v>79</v>
+      </c>
+      <c r="N2" s="37">
         <v>45557</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="14"/>
       <c r="G3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
       <c r="M3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="N3" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="M4" s="9" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
@@ -2296,21 +2616,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="G5" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
+      <c r="G5" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
       <c r="M5" s="8" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
@@ -2319,19 +2639,19 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
       <c r="M6" s="8" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
@@ -2340,17 +2660,17 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -2359,17 +2679,17 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -2378,21 +2698,21 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="G9" s="9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="M9" s="9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -2400,147 +2720,147 @@
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="35" t="s">
-        <v>103</v>
+      <c r="A10" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="40"/>
+      <c r="E10" s="32" t="s">
+        <v>90</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="J10" s="45"/>
+      <c r="G10" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="39"/>
       <c r="K10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="M10" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="P10" s="45"/>
+        <v>90</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="P10" s="39"/>
       <c r="Q10" s="10" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="36">
+      <c r="A11" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="E11" s="33">
         <v>45560</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
       <c r="K11" s="11"/>
-      <c r="M11" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="P11" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q11" s="27">
+      <c r="M11" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="22"/>
+      <c r="O11" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q11" s="24">
         <v>45560</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="36">
+      <c r="A12" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="44"/>
+      <c r="E12" s="33">
         <v>45560</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="11"/>
-      <c r="M12" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="P12" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q12" s="24">
+      <c r="M12" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="P12" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q12" s="21">
         <v>45560</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="36">
+      <c r="A13" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="33">
         <v>45560</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
       <c r="K13" s="11"/>
-      <c r="M13" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="P13" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q13" s="24">
+      <c r="M13" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="N13" s="19"/>
+      <c r="O13" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q13" s="21">
         <v>45560</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="36">
+      <c r="A14" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="33">
         <v>45560</v>
       </c>
       <c r="G14" s="8"/>
@@ -2548,137 +2868,137 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="M14" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="N14" s="25"/>
-      <c r="O14" s="26" t="s">
+      <c r="M14" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="22"/>
+      <c r="O14" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="P14" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="P14" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q14" s="27">
+      <c r="Q14" s="24">
         <v>45560</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="G16" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="M16" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
+      <c r="A16" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="G16" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="M16" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="43">
+        <v>79</v>
+      </c>
+      <c r="B17" s="37">
         <v>45558</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
       <c r="G17" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="43">
+        <v>79</v>
+      </c>
+      <c r="H17" s="37">
         <v>45559</v>
       </c>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
       <c r="M17" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="N17" s="43">
+        <v>79</v>
+      </c>
+      <c r="N17" s="37">
         <v>45560</v>
       </c>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
       <c r="G18" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
       <c r="M18" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="N18" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="O18" s="44"/>
-      <c r="P18" s="44"/>
-      <c r="Q18" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="N18" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="G19" s="9" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="M19" s="9" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
@@ -2686,106 +3006,106 @@
       <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="G20" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="M20" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
+      <c r="A20" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="M20" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="G21" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="M21" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
+      <c r="A21" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="M21" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
+      <c r="A22" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="G22" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="M24" s="9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
@@ -2793,207 +3113,207 @@
       <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>140</v>
+      <c r="A25" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="39"/>
+      <c r="C25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="H25" s="45"/>
-      <c r="I25" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>140</v>
+        <v>90</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="39"/>
+      <c r="I25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="M25" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="N25" s="45"/>
-      <c r="O25" s="21" t="s">
-        <v>102</v>
+        <v>90</v>
+      </c>
+      <c r="M25" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="N25" s="39"/>
+      <c r="O25" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="P25" s="10" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="Q25" s="10" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="21">
+        <v>45560</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="I26" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="K26" s="27">
+        <v>45560</v>
+      </c>
+      <c r="M26" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="P26" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="E26" s="24">
+      <c r="Q26" s="29">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="21">
         <v>45560</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G27" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="25"/>
+      <c r="I27" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="J27" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="K27" s="27">
+        <v>45560</v>
+      </c>
+      <c r="M27" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="P27" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="J26" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="K26" s="30">
+      <c r="Q27" s="29">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="24">
         <v>45560</v>
       </c>
-      <c r="M26" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="P26" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q26" s="32">
+      <c r="G28" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="25"/>
+      <c r="I28" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="K28" s="27">
+        <v>45560</v>
+      </c>
+      <c r="M28" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="P28" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q28" s="29">
         <v>45537</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="24">
-        <v>45560</v>
-      </c>
-      <c r="G27" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="J27" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="K27" s="30">
-        <v>45560</v>
-      </c>
-      <c r="M27" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="P27" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q27" s="32">
-        <v>45537</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="27">
-        <v>45560</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="J28" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="K28" s="30">
-        <v>45560</v>
-      </c>
-      <c r="M28" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="P28" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q28" s="32">
-        <v>45537</v>
-      </c>
-    </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="27">
+      <c r="A29" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="24">
         <v>45565</v>
       </c>
-      <c r="G29" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="J29" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="K29" s="30">
+      <c r="G29" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="K29" s="27">
         <v>45565</v>
       </c>
-      <c r="M29" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="P29" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q29" s="32">
+      <c r="M29" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="P29" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q29" s="29">
         <v>45537</v>
       </c>
     </row>
@@ -3009,72 +3329,46 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="M30" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="P30" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q30" s="34">
+      <c r="M30" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="P30" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q30" s="31">
         <v>45561</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
     </row>
     <row r="59" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R59" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G5:K8"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="G25:H25"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A11:B11"/>
@@ -3088,6 +3382,32 @@
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G5:K8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização do código da API
</commit_message>
<xml_diff>
--- a/documentacao/RequisitosPI.xlsx
+++ b/documentacao/RequisitosPI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_santos043_sptech_school/Documents/Projeto PI/projeto-pi-diesel-2/documentacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Gotardo\Desktop\Projeto\projeto-pi-diesel-2\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="13_ncr:1_{B83792C9-AA03-47B7-B1A9-83FE05156973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DCBC797-3F66-4D2A-AB94-97AD4F0C6EAF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0FB31F-D4BF-43A0-85EE-AD0957968E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="193">
   <si>
     <t>Requisito</t>
   </si>
@@ -763,12 +763,18 @@
   <si>
     <t>SPRINT 3</t>
   </si>
+  <si>
+    <t xml:space="preserve">Estilização da dashBoard com API funcionando </t>
+  </si>
+  <si>
+    <t>Área do site com acesso as DashBoards, já com estilização final</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,6 +851,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -959,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1049,42 +1062,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1100,6 +1077,45 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1484,11 +1500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1505,527 +1521,527 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="35" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="49" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="49" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="49" t="s">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="49" t="s">
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
     </row>
     <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="49" t="s">
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="49" t="s">
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="49" t="s">
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="49" t="s">
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="49" t="s">
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="49" t="s">
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="49" t="s">
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="49" t="s">
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="49" t="s">
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
     </row>
     <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="49" t="s">
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
     </row>
     <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="49" t="s">
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
     </row>
     <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="49" t="s">
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
     </row>
     <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="49" t="s">
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
     </row>
     <row r="20" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="49" t="s">
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="49" t="s">
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="49" t="s">
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="49" t="s">
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
     </row>
     <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="49" t="s">
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
     </row>
     <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="49" t="s">
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
     </row>
     <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="49" t="s">
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
       <c r="G27" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
     </row>
     <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="37" t="s">
         <v>188</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -2036,10 +2052,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="39" t="s">
         <v>189</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -2048,6 +2064,23 @@
       <c r="G29" s="2" t="s">
         <v>190</v>
       </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G31" s="53"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:I2" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}"/>
@@ -2107,7 +2140,7 @@
       <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="42" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2130,7 +2163,7 @@
       <c r="F2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="35"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2508,88 +2541,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="12"/>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="M1" s="36" t="s">
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="M1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="46">
         <v>45554</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="13"/>
       <c r="G2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="46">
         <v>45555</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="M2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="37">
+      <c r="N2" s="46">
         <v>45557</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="14"/>
       <c r="G3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
       <c r="M3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -2622,13 +2655,13 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
       <c r="M5" s="8" t="s">
         <v>107</v>
       </c>
@@ -2645,11 +2678,11 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
       <c r="M6" s="8" t="s">
         <v>108</v>
       </c>
@@ -2666,11 +2699,11 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -2685,11 +2718,11 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -2720,58 +2753,58 @@
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40" t="s">
+      <c r="B10" s="52"/>
+      <c r="C10" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="32" t="s">
         <v>90</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39" t="s">
+      <c r="H10" s="50"/>
+      <c r="I10" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="39"/>
+      <c r="J10" s="50"/>
       <c r="K10" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39" t="s">
+      <c r="N10" s="50"/>
+      <c r="O10" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="P10" s="39"/>
+      <c r="P10" s="50"/>
       <c r="Q10" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="33">
         <v>45560</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
       <c r="K11" s="11"/>
       <c r="M11" s="22" t="s">
         <v>91</v>
@@ -2788,22 +2821,22 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="44"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="33">
         <v>45560</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="11"/>
       <c r="M12" s="19" t="s">
         <v>92</v>
@@ -2820,22 +2853,22 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="44"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="33">
         <v>45560</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="11"/>
       <c r="M13" s="19" t="s">
         <v>93</v>
@@ -2852,14 +2885,14 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="44"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="33">
         <v>45560</v>
       </c>
@@ -2902,85 +2935,85 @@
       <c r="Q15" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="G16" s="36" t="s">
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="G16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="M16" s="36" t="s">
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="M16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="37">
+      <c r="B17" s="46">
         <v>45558</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
       <c r="G17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="46">
         <v>45559</v>
       </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
       <c r="M17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N17" s="37">
+      <c r="N17" s="46">
         <v>45560</v>
       </c>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="G18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="38" t="s">
+      <c r="H18" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
       <c r="M18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="38" t="s">
+      <c r="N18" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
@@ -3113,10 +3146,10 @@
       <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="39"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="18" t="s">
         <v>89</v>
       </c>
@@ -3126,10 +3159,10 @@
       <c r="E25" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="39"/>
+      <c r="H25" s="50"/>
       <c r="I25" s="18" t="s">
         <v>89</v>
       </c>
@@ -3139,10 +3172,10 @@
       <c r="K25" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="M25" s="39" t="s">
+      <c r="M25" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="N25" s="39"/>
+      <c r="N25" s="50"/>
       <c r="O25" s="18" t="s">
         <v>89</v>
       </c>
@@ -3369,6 +3402,32 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G5:K8"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A11:B11"/>
@@ -3382,32 +3441,6 @@
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G5:K8"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>